<commit_message>
Add task evidence A1-B7
</commit_message>
<xml_diff>
--- a/DreamGallery/evidence.xlsx
+++ b/DreamGallery/evidence.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\25114\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\25114\Downloads\DreamGallery\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA9AECBE-0F09-4062-9DF6-8F27A3BA84C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AF7F610-2E27-4D29-818A-BE481F5DA413}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5220" yWindow="345" windowWidth="21600" windowHeight="14040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4890" yWindow="885" windowWidth="21600" windowHeight="14040" firstSheet="14" activeTab="25" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -38,65 +38,28 @@
     <sheet name="B2" sheetId="23" r:id="rId23"/>
     <sheet name="B5" sheetId="24" r:id="rId24"/>
     <sheet name="B6" sheetId="25" r:id="rId25"/>
+    <sheet name="B7" sheetId="27" r:id="rId26"/>
+    <sheet name="Sheet1" sheetId="26" r:id="rId27"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="96">
   <si>
     <t>TxHash</t>
   </si>
   <si>
-    <t>The first Interchain NFT-Transfer TxHash</t>
-  </si>
-  <si>
-    <t>The Internal Transfer TxHash on IRISnet</t>
-  </si>
-  <si>
     <t>ChainID</t>
   </si>
   <si>
-    <t>tx hash on that chain</t>
-  </si>
-  <si>
-    <t>chain id</t>
-  </si>
-  <si>
-    <t>tx hash on that chain	chain id</t>
-  </si>
-  <si>
     <t>ClassID</t>
   </si>
   <si>
     <t>NFTID</t>
   </si>
   <si>
-    <t>ibc class on chain</t>
-  </si>
-  <si>
-    <t>nft id</t>
-  </si>
-  <si>
-    <t>tx hash on dest chain</t>
-  </si>
-  <si>
-    <t>dest chain id</t>
-  </si>
-  <si>
-    <t>tx hash on irisnet</t>
-  </si>
-  <si>
-    <t>ibc class on dest chain</t>
-  </si>
-  <si>
-    <t>class id you issued</t>
-  </si>
-  <si>
-    <t>nft id you minted</t>
-  </si>
-  <si>
     <t>TeamName</t>
   </si>
   <si>
@@ -150,6 +113,310 @@
   </si>
   <si>
     <t>DreamGallery#9700</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>53801A26FCAD70F4AC1D3C875C6E9F7A0EB4CC12BCFF412F92325B735A7FA338</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>tegon</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>3E612BF99F3FC8E90121D73160A0BDAD9B83CDDEA0683CA0CDAE7EDBAB72D94D</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>gameofNFT001</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>FB8E84F2263A6C573E174288563D9DFD89CA6A6A0A1780C80C30F6C859335729</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>gameofNFT002</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>AD4830FEA4DF6D4A9780706FE1689C5CAA0EB72736B73DA6EB20689ACD3266BB</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>elgafar-1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>E06EA059CCEA6AEC2A68A83CA41B8693473532332EDA878C641F7DE075F8E190</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>uptick_7000-2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ibc/0709674605B3B0F837A72BE57F83CFF0ABB85765F59524708C8B53CBEF18B97B</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>D73962B517B03E402B4EC407C0EE040CBF78CAD73252E4D32795A52201598354</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>gon-irishub-1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>stars1uml8uhqdc27c8dl3tty0vgyrc9yvnz0qjq5faulhpzfw03kz6tmqpqje24</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C0C2BF1A532C4483A3577C5B3ED40700E35A5271E2E0C882B1716A859C1E3165</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>gameofNFTa1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ibc/BEE8EE6AB4AD05AABBE56CC40A6E5D9EF6DD3D19BA0996D6113BDC74BEC02B37</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ibc/B2B9E519D42A97E0B659943D6CBB227133FE45D51E746138A407EDA1BEF17AE6</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>gameofNFTa2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ibc/E59D2644DB072BE4FF7BEEE1F3D6F0BD05C8E30A94C69AB4206C6EF89193060C</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>gameofNFTa3</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ibc/B584337B2C4AF103EFB13432282F8E6A299E15FA06109E0BE66B4D04A3471A26</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>gameofNFTa4</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ibc/0E5BF61B256E277EB32BA400D5F3AE563FEDBFA5DE8DB4F320A8F8AF6175AAF1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>gameofNFTa5</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ibc/6066376149F96EB857263FD8D97D3800C6D0515B859C4F3D0CDEA141A73520E6</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>gameofNFTa6of2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>4B0DD06C4FF25F9F24561AD9737C8C4302CC8C9FF2C0A8071F4209E0CB73D01C</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>BF3041F375053296397008CB42ECEA76FF95F1FFAC0D6D957552911C67542759</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>DA828A8D769B8A184416A9996E74865FEA11E0AD6289228615B5B658A4CE6DE1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>FA06933A74F78246C7F7D74579CF1825BE27D17A3E84E0EA08B87DF501C5F735</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>274B8773AB202BAEDFCF0E21C02B4D61AD7E02BDB5615AF4B8BD95F95A301CB7</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1D67307D80789F6689C2DC78C958BF03D33BB398594B0014BB99E4E058E4C81F</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>94E5574206F9ACC7274242EF46A64314467053C6465731C6680586264DB387E0</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>gon-flixnet-1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>30031978E8E360CB38D1743C112A6DF35F61E5AA207DFDBF7347807D2CD03F67</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>uni-6</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>32EE87CABB0EE76CD0544B57A3E2633F348CF0B45A6738C437B2892AA5624FF4</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>60AB409950737755ADA2425F995F7954F248517F03426D486CAD67E98252D27E</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1C082F2402657C13ED1A43E84561B0D58675E2B82C9B0DD46AC8B69401773EB9</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0AA38428AF48A069294E9587C62AC63B24838CC10303B4562661951647FAC7C2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>842DE161DABB6E1B76386AEB2829CEC9379AB3E82CA819F83AAA4653879D534F</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>FA04FA70D0691DE3682B73BD8D4F08B3930CDD3352C647369E6FFB90923AB5FC</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>3D9115647EF3348252C630D59E06249D6763AD0E5D82D1545CF4E969B92F5E50</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>F648E773151109203485191B947C60F1389675A96CED98137316A2030230FFEC</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>TxHash</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>153E6DF8A8F1FC4C254A415DBAB7BD7CB76A1D16074AF3472ED26CE320912C2D</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>FDEF8303FD55439BC6E0BD1448904006C6CB6BA1822CC227DDB7F8C6A5FF465B</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>6FF6E4877E255051A2BAEEE12FE1E93DD347A465341CA6E959B9518ADD733D86</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>53A84A33BF6FDD3EB5040B0D5C3950DEB3B5D3A2C48AC4AC5A195BE99F9F7D8A</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0A3D808610F48B08B8166D9DD4B6D1898F0B14DB68A703E24E2A584903519D13</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0D78F516B439FEB2E3A2ADB3251AD0B95816B21A214F45E7135EC918D346311D</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>80297F1EF7933CE1440B931720E306F6DEE7C44857DB6DCC5EF67BBE9CB5E90C</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>472A19B7286E6E8E34F0DF4FC1B5544A009BD9D25915DA92214EE9BC04C8E9B7</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>D51D87834FF3B0F78675519739F66682DCA8A4752FE1AE4CA3233BC0C823F9E5</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>7666F606608A9E18F2201DE04D057EA48873E5239937106FCC9FD6698FE5E1B4</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>AF9BFC5FF8E4AF27DF0EDDECDF2F6065802D83BDC2C889EFF8B808563EF4C4C7</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>899D318F658401856B46864E5A0993E25EE2060A4B1508EC14FD0B7F26528088</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>87DF06F57F239A82567C98388B05C98FC3474D470EF3A940D38C88B8736F59E7</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>B792D323CB7D8FD5CB784EBEDA65ABA3143D449E7237A9E7BDCE4C4A29748F48</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>BC1A293BFFF4CA9191A20BA4F77196F44E65EB581656CB6BBD6CDE73D23328CF</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>229D1B59DD35B213F94FB517C81A05F8A2EE44EFE8B902E04259B9DC92AE5938</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>EBC85C0C962F350632DE8FB7321E33C880B4FD91EC1D962A9DC0A2E4D91F36BD</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1AC9826618A5370FB8A684692F3C1C8377AFDD647FE20DD42B16658DD6ABA8DC</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C73856B67F5907B608E017063BBC402C7F453B5BB65639A7872867EE9D24C83F</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>DCE121F889E0288DA84CD38507841E2C830FFD4B0A46F1D8BA3125265509A3C5</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ADEEC928D1E9FBA1DAEC085B050D523AA60FD7C07BA4501367F980063AF7BC31</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CCED0ABDC63856CCF8A40F913B257E9EECF87208E253C0DBB51B5CA049B47626</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>A9A7B54D64ABDBB509231BD473E0E319BF2DB2DC6E3EE61F3AA1E395E8854BBE</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C1C7546DCBEE3880176C2D612950C2FA9BD124D9738D72271435722500B91C62</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ED376822FB8579EC41E232308BB530BDD7F04B7CB045D1B24C0E8B1EABADB815</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>B7EC42A716E2A7812562B40DF29AF804ED7EA33AA68D217674B5AA292F812D76</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>D44C7EC93659C6782E1C7DCAF946ADCB56843209B4DC1BFA16C2A67B93409848</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>D334779ABF0F1B394FD3585290CBE0C2305D7A2D3E73DFDF7E19295036F297DA</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>D26A5E645CD631899D912170330065670B98A73761A7F05E197EAC6893E0849D</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>F97F369178010B57DF28F8D7B46CE9D0B111D76762EA2528EB48A9A417692848</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -157,7 +424,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -177,6 +444,12 @@
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -231,7 +504,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -243,6 +516,10 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -552,8 +829,8 @@
   </sheetPr>
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -570,54 +847,54 @@
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="H2" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -633,7 +910,9 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
@@ -643,34 +922,216 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>47</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
@@ -680,34 +1141,60 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>51</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
@@ -717,34 +1204,60 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
@@ -754,34 +1267,60 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>61</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
@@ -791,44 +1330,60 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>65</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>66</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>67</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+        <v>68</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
@@ -841,41 +1396,95 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>70</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>71</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+        <v>72</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="2" width="17.875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
@@ -888,41 +1497,73 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>74</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>75</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+        <v>76</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
@@ -935,249 +1576,55 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>80</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>81</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="1" max="2" width="17.875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>82</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1193,7 +1640,9 @@
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
@@ -1207,12 +1656,12 @@
     </row>
     <row r="2" spans="1:1" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>2</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -1228,7 +1677,9 @@
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
@@ -1242,12 +1693,12 @@
     </row>
     <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>2</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -1263,7 +1714,9 @@
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
@@ -1277,12 +1730,12 @@
     </row>
     <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>2</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -1298,7 +1751,9 @@
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
@@ -1312,15 +1767,65 @@
     </row>
     <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
+        <v>93</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0942ECC4-6CB0-498F-87BE-900C9142AA9A}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="12.375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34C1E636-8384-4032-AEA1-766854B27459}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1331,9 +1836,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
@@ -1346,21 +1853,32 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>16</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -1376,7 +1894,9 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
@@ -1390,27 +1910,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>12</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -1426,7 +1946,9 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
@@ -1440,27 +1962,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>12</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1476,7 +1998,9 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
@@ -1490,27 +2014,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>12</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1526,7 +2050,9 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
@@ -1541,27 +2067,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>12</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1577,7 +2103,9 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
@@ -1587,18 +2115,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1614,7 +2142,9 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
@@ -1624,18 +2154,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>